<commit_message>
PC ORD data files
</commit_message>
<xml_diff>
--- a/PC-ORD/Original Data/diets2.xlsx
+++ b/PC-ORD/Original Data/diets2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedar\Documents\GitHub\Thesis\PC-ORD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedar\Documents\GitHub\Thesis\PC-ORD\Original Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFA51FF-2E12-463F-930A-A743C53286DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813A634C-ECF5-4D25-A410-506ECE2DA422}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Stream</t>
   </si>
@@ -62,6 +62,24 @@
   </si>
   <si>
     <t>W-113 2</t>
+  </si>
+  <si>
+    <t>CHUCK</t>
+  </si>
+  <si>
+    <t>LOON</t>
+  </si>
+  <si>
+    <t>MCTE</t>
+  </si>
+  <si>
+    <t>W-100</t>
+  </si>
+  <si>
+    <t>W-113</t>
+  </si>
+  <si>
+    <t>RowName</t>
   </si>
 </sst>
 </file>
@@ -902,99 +920,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>